<commit_message>
Adds rsp data as well to free agent
</commit_message>
<xml_diff>
--- a/python_analysis/data/common/Reception_Perception_Dynasty.xlsx
+++ b/python_analysis/data/common/Reception_Perception_Dynasty.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28827"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/28a1ee50a88aa706/python_work/Dynasty_tools/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/28a1ee50a88aa706/python_work/volatile/python_analysis/data/common/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="31" documentId="8_{389A4676-7C93-4697-AA30-3844E99EB7A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{61E64332-BF40-4A8A-8A7B-6E13ACCA717F}"/>
+  <xr:revisionPtr revIDLastSave="32" documentId="8_{389A4676-7C93-4697-AA30-3844E99EB7A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{767A18E9-BD86-4201-ADEF-526DF9B42EF7}"/>
   <bookViews>
-    <workbookView xWindow="2660" yWindow="2660" windowWidth="28800" windowHeight="15460" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2280" yWindow="2280" windowWidth="28800" windowHeight="15460" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -851,10 +851,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1185,7 +1181,7 @@
     <col min="1" max="1" width="11.08984375" customWidth="1"/>
     <col min="2" max="2" width="32.36328125" customWidth="1"/>
     <col min="3" max="3" width="13.453125" customWidth="1"/>
-    <col min="4" max="4" width="41.1796875" customWidth="1"/>
+    <col min="4" max="4" width="81.1796875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="72.54296875" customWidth="1"/>
     <col min="6" max="6" width="17.54296875" customWidth="1"/>
   </cols>

</xml_diff>